<commit_message>
fix: too many fetch to create req_order
</commit_message>
<xml_diff>
--- a/temp/test.xlsx
+++ b/temp/test.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="23">
   <si>
     <t>หัวตารางแจ้งงาน</t>
   </si>
@@ -414,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -658,6 +658,270 @@
         <v>22</v>
       </c>
     </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="1">
+        <v>110302</v>
+      </c>
+      <c r="E6" s="1">
+        <v>110302</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="1">
+        <v>25</v>
+      </c>
+      <c r="H6" s="1">
+        <v>110302106</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M6" s="1">
+        <v>2568</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="1">
+        <v>110302</v>
+      </c>
+      <c r="E7" s="1">
+        <v>110302</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="1">
+        <v>25</v>
+      </c>
+      <c r="H7" s="1">
+        <v>110302106</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M7" s="1">
+        <v>2568</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="1">
+        <v>110302</v>
+      </c>
+      <c r="E8" s="1">
+        <v>110302</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="1">
+        <v>25</v>
+      </c>
+      <c r="H8" s="1">
+        <v>110302106</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M8" s="1">
+        <v>2568</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="1">
+        <v>110302</v>
+      </c>
+      <c r="E9" s="1">
+        <v>110302</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" s="1">
+        <v>25</v>
+      </c>
+      <c r="H9" s="1">
+        <v>110302106</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M9" s="1">
+        <v>2568</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="1">
+        <v>110302</v>
+      </c>
+      <c r="E10" s="1">
+        <v>110302</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" s="1">
+        <v>25</v>
+      </c>
+      <c r="H10" s="1">
+        <v>110302106</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M10" s="1">
+        <v>2568</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="1">
+        <v>110302</v>
+      </c>
+      <c r="E11" s="1">
+        <v>110302</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" s="1">
+        <v>25</v>
+      </c>
+      <c r="H11" s="1">
+        <v>110302106</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M11" s="1">
+        <v>2568</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>